<commit_message>
revision accuracy & output accuracy
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Directory Information</t>
   </si>
@@ -25,13 +25,16 @@
     <t>Personally Identifiable</t>
   </si>
   <si>
-    <t>Accuracy Website = 8.33%</t>
+    <t>Akurasi Pengujian = 8.80%</t>
   </si>
   <si>
     <t>Indikator</t>
   </si>
   <si>
     <t>Data</t>
+  </si>
+  <si>
+    <t>Akurasi</t>
   </si>
   <si>
     <t>Nama Institusi</t>
@@ -83,6 +86,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00%"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -112,9 +118,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -430,185 +439,258 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="I2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1">
+        <v>252</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.5187007874015748</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
       <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="E7" t="s">
+        <v>252</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.5187007874015748</v>
+      </c>
+      <c r="G6" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="E8" t="s">
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="G7" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="E9" t="s">
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="G8" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1">
+        <v>214</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.421259842519685</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1">
         <f>SUM(B1:B7)</f>
         <v>0</v>
       </c>
-      <c r="D10" s="1">
-        <f>SUM(D1:D7)</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <f>SUM(F1:F7)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1" t="s">
+      <c r="C10" s="2">
+        <f>AVERAGE(C1:C7)</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <f>SUM(E1:E7)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <f>AVERAGE(F1:F7)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <f>SUM(H1:H9)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <f>AVERAGE(I1:I9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A11:I11"/>
   </mergeCells>
-  <conditionalFormatting sqref="A12:F12">
+  <conditionalFormatting sqref="A11:I11">
     <cfRule type="notContainsBlanks" dxfId="0" priority="3">
-      <formula>LEN(TRIM(A12))&gt;0</formula>
+      <formula>LEN(TRIM(A11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:F10">
+  <conditionalFormatting sqref="A1:I10">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
add keywords and add more tables in website 8
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -25,7 +25,7 @@
     <t>Personally Identifiable</t>
   </si>
   <si>
-    <t>Akurasi Pengujian = 0.00%</t>
+    <t>Akurasi Pengujian = 32.73%</t>
   </si>
   <si>
     <t>Indikator</t>
@@ -519,10 +519,10 @@
         <v>14</v>
       </c>
       <c r="H3" s="1">
-        <v>0</v>
+        <v>1001</v>
       </c>
       <c r="I3" s="2">
-        <v>0</v>
+        <v>0.8833786231884058</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -548,10 +548,10 @@
         <v>15</v>
       </c>
       <c r="H4" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -559,19 +559,19 @@
         <v>9</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>433</v>
       </c>
       <c r="F5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
         <v>16</v>
@@ -619,10 +619,10 @@
         <v>19</v>
       </c>
       <c r="H8" s="1">
-        <v>0</v>
+        <v>472</v>
       </c>
       <c r="I8" s="2">
-        <v>0</v>
+        <v>0.90625</v>
       </c>
     </row>
     <row r="9" spans="1:9">

</xml_diff>